<commit_message>
verified tuning corrector gas mixture intensity correction
updated tuning corrector gas mixture readme
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
+++ b/UnitTests/TuningCorrectorGasMixture/TuningCorrectorGasMixtureHypotheticalReferenceMeasuredVsSimulated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\ExampleTuningCorrectorGasMixture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvs\Documents\GitHub\MSRESOLVESG\UnitTests\TuningCorrectorGasMixture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5270E44C-D4FB-4B45-9261-0883841DED09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257EA9F2-FCC0-4753-8BE4-F9F23DB8474F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Removing m17 m21 and m22</t>
   </si>
   <si>
-    <t>Simulated</t>
-  </si>
-  <si>
     <t>Meas x 1E8 / 140</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>So the Mixed Reference Pattern coming out is as expected.</t>
+  </si>
+  <si>
+    <t>Simulated from Literature Patterns</t>
   </si>
 </sst>
 </file>
@@ -2642,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,28 +2659,28 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>0.69541048019294749</v>
       </c>
       <c r="T2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>0.61389505114073639</v>
       </c>
       <c r="T4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -2837,13 +2837,13 @@
         <v>0.58675606160212657</v>
       </c>
       <c r="T5" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" t="s">
         <v>13</v>
       </c>
-      <c r="U5" t="s">
-        <v>14</v>
-      </c>
       <c r="V5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>0.75106690537950227</v>
       </c>
       <c r="T7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2967,13 +2967,13 @@
         <v>0.8147194157575286</v>
       </c>
       <c r="T8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" t="s">
         <v>13</v>
       </c>
-      <c r="U8" t="s">
-        <v>14</v>
-      </c>
       <c r="V8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>0.96926188648857314</v>
       </c>
       <c r="T10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -3139,7 +3139,7 @@
         <v>1.1601209571862721</v>
       </c>
       <c r="T12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -3178,13 +3178,13 @@
         <v>1.269169217522617</v>
       </c>
       <c r="T13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" t="s">
         <v>13</v>
       </c>
-      <c r="U13" t="s">
-        <v>14</v>
-      </c>
       <c r="V13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -3210,23 +3210,23 @@
         <v>6.4249909515011829</v>
       </c>
       <c r="W14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="T15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="T16" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" t="s">
         <v>13</v>
       </c>
-      <c r="U16" t="s">
-        <v>14</v>
-      </c>
       <c r="V16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="20:22" x14ac:dyDescent="0.25">
@@ -3243,7 +3243,7 @@
     </row>
     <row r="18" spans="20:22" x14ac:dyDescent="0.25">
       <c r="T18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>